<commit_message>
Get Driver Test cases updated
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/API_TestData.xlsx
+++ b/src/test/java/TestData/API_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\taxi-booking-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45E788C-06CC-4F13-8854-BEF9342F033C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F6473C-60CD-4318-8505-B1A4D83C8D35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query_Parm" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>Key</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>driver.test_43@gmail.com</t>
+  </si>
+  <si>
+    <t>7755663245</t>
+  </si>
+  <si>
+    <t>driver.test_45@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -898,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA34F427-6D3C-4F27-A42C-B9885A0ABD9F}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -938,7 +944,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -946,7 +952,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1026,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DA1B3F-A3AE-4A2A-B3AC-AAEA5516112C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
Deserilize Test Case Updated
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/API_TestData.xlsx
+++ b/src/test/java/TestData/API_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\taxi-booking-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F6473C-60CD-4318-8505-B1A4D83C8D35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD06423-3FE4-4BCE-892B-57BDAE0AA6C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query_Parm" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>Key</t>
   </si>
@@ -145,16 +145,10 @@
     <t>username</t>
   </si>
   <si>
-    <t>7755663243</t>
-  </si>
-  <si>
-    <t>driver.test_43@gmail.com</t>
-  </si>
-  <si>
-    <t>7755663245</t>
-  </si>
-  <si>
-    <t>driver.test_45@gmail.com</t>
+    <t>7755663251</t>
+  </si>
+  <si>
+    <t>driver.test_51@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -904,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA34F427-6D3C-4F27-A42C-B9885A0ABD9F}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -944,7 +938,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -952,7 +946,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1032,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DA1B3F-A3AE-4A2A-B3AC-AAEA5516112C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
PATCH Request for Driver Location PINCODE
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/API_TestData.xlsx
+++ b/src/test/java/TestData/API_TestData.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\taxi-booking-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD06423-3FE4-4BCE-892B-57BDAE0AA6C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A72D0E8-9B08-4BF8-B0B0-AD554008064D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query_Parm" sheetId="1" r:id="rId1"/>
     <sheet name="Get_JsonResponse" sheetId="2" r:id="rId2"/>
     <sheet name="driver_Post" sheetId="5" r:id="rId3"/>
     <sheet name="driver_verify_Post" sheetId="7" r:id="rId4"/>
-    <sheet name="driver_Post_ValidationData" sheetId="6" r:id="rId5"/>
-    <sheet name="Post_Req" sheetId="3" r:id="rId6"/>
-    <sheet name="Patch_Req" sheetId="4" r:id="rId7"/>
+    <sheet name="driver_LocPinCode" sheetId="8" r:id="rId5"/>
+    <sheet name="driver_Post_ValidationData" sheetId="6" r:id="rId6"/>
+    <sheet name="Post_Req" sheetId="3" r:id="rId7"/>
+    <sheet name="Patch_Req" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>Key</t>
   </si>
@@ -145,10 +146,13 @@
     <t>username</t>
   </si>
   <si>
-    <t>7755663251</t>
-  </si>
-  <si>
-    <t>driver.test_51@gmail.com</t>
+    <t>400706</t>
+  </si>
+  <si>
+    <t>7755668283</t>
+  </si>
+  <si>
+    <t>driver.test_83@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -938,7 +942,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -946,7 +950,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -980,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302FC2D0-A276-48F1-B10C-083CF1C437DE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1002,7 +1006,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1023,10 +1027,56 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEE180F-E3F5-4F4E-89EA-4DE3CE903CE9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="Admin@demo" xr:uid="{F6A85FF9-02F9-4D4D-8C31-3057BC619F94}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DA1B3F-A3AE-4A2A-B3AC-AAEA5516112C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1123,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1081,7 +1131,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1104,8 +1154,8 @@
       <c r="A9" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="36">
-        <v>400706</v>
+      <c r="B9" s="36" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1134,7 +1184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0551401-394D-415A-AC53-C7789C67DA93}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1223,7 +1273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE7AF6A-85FD-4F61-B0FC-C1E3E316E178}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Passenger Registeration Test Cases added
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/API_TestData.xlsx
+++ b/src/test/java/TestData/API_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\taxi-booking-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A72D0E8-9B08-4BF8-B0B0-AD554008064D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD19168-F5A9-4D3B-AF32-E9AA31477056}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query_Parm" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="driver_Post" sheetId="5" r:id="rId3"/>
     <sheet name="driver_verify_Post" sheetId="7" r:id="rId4"/>
     <sheet name="driver_LocPinCode" sheetId="8" r:id="rId5"/>
-    <sheet name="driver_Post_ValidationData" sheetId="6" r:id="rId6"/>
-    <sheet name="Post_Req" sheetId="3" r:id="rId7"/>
-    <sheet name="Patch_Req" sheetId="4" r:id="rId8"/>
+    <sheet name="driverChangePWD_Post" sheetId="9" r:id="rId6"/>
+    <sheet name="driver_Post_ValidationData" sheetId="6" r:id="rId7"/>
+    <sheet name="Post_Req" sheetId="3" r:id="rId8"/>
+    <sheet name="Patch_Req" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -149,10 +150,16 @@
     <t>400706</t>
   </si>
   <si>
-    <t>7755668283</t>
-  </si>
-  <si>
-    <t>driver.test_83@gmail.com</t>
+    <t>oldPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>7755668292</t>
+  </si>
+  <si>
+    <t>driver.test_92@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -291,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,6 +377,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -942,7 +956,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -950,7 +964,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -984,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302FC2D0-A276-48F1-B10C-083CF1C437DE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1006,7 +1020,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1052,7 +1066,7 @@
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="40" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1073,8 +1087,59 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB14D14B-B935-458C-BAA2-EADEE30037E8}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{7B276DC7-7E93-4610-B806-C2B07709A42C}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8A513667-CFEE-4FDF-845D-CFCBB6EB6A46}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DA1B3F-A3AE-4A2A-B3AC-AAEA5516112C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1086,7 +1151,7 @@
     <col min="2" max="2" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="36" t="s">
         <v>29</v>
       </c>
@@ -1102,7 +1167,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="34" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="34" t="s">
         <v>21</v>
       </c>
@@ -1118,23 +1183,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="34" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="34" t="s">
         <v>26</v>
       </c>
@@ -1142,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" s="36" t="s">
         <v>30</v>
       </c>
@@ -1150,7 +1215,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" s="36" t="s">
         <v>31</v>
       </c>
@@ -1158,15 +1223,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="36" t="s">
         <v>33</v>
       </c>
@@ -1178,13 +1246,14 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="Admin@123" xr:uid="{8D030A28-CD16-478B-A8AC-861204221E3A}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{70A28AD4-D364-410C-A042-2437C58D0917}"/>
+    <hyperlink ref="B10" r:id="rId3" display="Admin@demo" xr:uid="{0EBCAC7E-F837-40B6-895D-580741C05DCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0551401-394D-415A-AC53-C7789C67DA93}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1273,7 +1342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE7AF6A-85FD-4F61-B0FC-C1E3E316E178}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>